<commit_message>
feat: se realizo la tarea recordar a los pacientes su turno
</commit_message>
<xml_diff>
--- a/service/ExcelHandler/turnos.xlsx
+++ b/service/ExcelHandler/turnos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\botwhat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Documentos\botwhat\service\ExcelHandler\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>fecha</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Lic. Peralta</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>Francisco</t>
   </si>
 </sst>
 </file>
@@ -77,7 +83,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -100,11 +106,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -123,6 +140,7 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,7 +432,7 @@
     <col min="1" max="1" width="22" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -427,8 +445,11 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="10" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>5493804937533</v>
       </c>
@@ -442,7 +463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -456,7 +477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>5493804275648</v>
       </c>
@@ -470,18 +491,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
-        <v>5493804229016</v>
+        <v>5493804401611</v>
       </c>
       <c r="B5" s="4">
-        <v>45807</v>
+        <v>45819</v>
       </c>
       <c r="C5" s="5">
         <v>0.89583333333333337</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>